<commit_message>
Added Images and some excel stuff
</commit_message>
<xml_diff>
--- a/Table/Classification Report Result.xlsx
+++ b/Table/Classification Report Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Islam\OneDrive\Documents\GitHub\Skripsi\Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9BEA75-AD5D-49E3-B882-1D9B286C929D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBA72F1-208F-4BFE-B947-9C0AE9E1688F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9A3E8AE5-FB14-4923-BBE8-3E26189E36AA}"/>
   </bookViews>
@@ -80,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -103,15 +103,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -119,6 +153,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -438,7 +481,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E4"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,131 +490,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>-1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0.73</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>0.76</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>0.75</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.72</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>0.48</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.63</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>0.83</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>0.72</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.68</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3">
+        <v>300</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="C6" s="3">
         <v>0.68</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="2">
+      <c r="D6" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="E6" s="3">
         <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
         <v>0.69</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>0.68</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>0.67</v>
       </c>
-      <c r="E7" s="2">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.69</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.68</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="E7" s="1">
         <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>